<commit_message>
12V to 5V LDO version
</commit_message>
<xml_diff>
--- a/LED_Ring/Production_Files/BOM-LESRv1.0.xlsx
+++ b/LED_Ring/Production_Files/BOM-LESRv1.0.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eagle_projects_directory\Florian_PCB\LED_Ring\Production_Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4403AB3-90F8-4044-8D3C-7E79A9DC3919}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20037955-48D6-4DEC-87A7-D4A01869BC97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,9 +199,6 @@
     <t>8-SMD Module</t>
   </si>
   <si>
-    <t>https://www.digikey.in/short/zmbq8t</t>
-  </si>
-  <si>
     <t>SOT-223</t>
   </si>
   <si>
@@ -238,18 +235,6 @@
     <t>https://www.digikey.in/short/zmbqvc</t>
   </si>
   <si>
-    <t>IN_1, IN_2, OUT_1,OUT_2</t>
-  </si>
-  <si>
-    <t>QWIIC COMPATIBLE JST SH 4PIN CON</t>
-  </si>
-  <si>
-    <t>Sparkfun</t>
-  </si>
-  <si>
-    <t>PRT-14417</t>
-  </si>
-  <si>
     <t xml:space="preserve">SMD </t>
   </si>
   <si>
@@ -259,9 +244,6 @@
     <t>RES SMD 4.7K OHM 5% 1/10W 0603</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.tanotis.com/products/sparkfun-qwiic-jst-connector-smd-4-pin </t>
-  </si>
-  <si>
     <t>https://www.digikey.in/short/zmb83b</t>
   </si>
   <si>
@@ -293,6 +275,24 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.digikey.in/short/z4hjwh </t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>S6B-PH-SM4-TB(LF)(SN)</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD R/A 6POS 2MM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/short/z98b8r</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.digikey.in/short/zmbq8t </t>
+  </si>
+  <si>
+    <t>IN</t>
   </si>
 </sst>
 </file>
@@ -890,7 +890,7 @@
   <dimension ref="A2:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8"/>
@@ -898,7 +898,7 @@
     <col min="1" max="1" width="9" style="3"/>
     <col min="2" max="2" width="43.88671875" style="3" customWidth="1"/>
     <col min="3" max="3" width="9" style="3"/>
-    <col min="4" max="4" width="21.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" style="3" customWidth="1"/>
     <col min="5" max="5" width="29.88671875" style="3" customWidth="1"/>
     <col min="6" max="6" width="41.6640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="20.88671875" style="3" customWidth="1"/>
@@ -984,8 +984,8 @@
       <c r="H7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="19" t="s">
-        <v>24</v>
+      <c r="I7" s="37" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:9" s="1" customFormat="1" ht="14.4">
@@ -1008,13 +1008,13 @@
         <v>13</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" s="18" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.4">
@@ -1022,7 +1022,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7">
         <v>10</v>
@@ -1031,19 +1031,19 @@
         <v>15</v>
       </c>
       <c r="E9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="G9" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>29</v>
       </c>
       <c r="H9" s="18" t="s">
         <v>9</v>
       </c>
       <c r="I9" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="41.4">
@@ -1051,57 +1051,57 @@
         <v>4</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="26">
         <v>14</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="27">
         <v>1655</v>
       </c>
       <c r="F10" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="28" t="s">
         <v>34</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>35</v>
       </c>
       <c r="H10" s="18" t="s">
         <v>9</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="14.4">
       <c r="A11" s="11">
         <v>5</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>37</v>
+        <v>55</v>
       </c>
       <c r="C11" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="H11" s="18" t="s">
         <v>9</v>
       </c>
       <c r="I11" s="29" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="14.4">
@@ -1109,7 +1109,7 @@
         <v>6</v>
       </c>
       <c r="B12" s="33" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C12" s="31">
         <v>1</v>
@@ -1118,19 +1118,19 @@
         <v>16</v>
       </c>
       <c r="E12" s="34" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="F12" s="38" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G12" s="36" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="H12" s="35" t="s">
         <v>9</v>
       </c>
       <c r="I12" s="37" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="14.4">
@@ -1138,7 +1138,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C13" s="7">
         <v>3</v>
@@ -1147,19 +1147,19 @@
         <v>16</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="G13" s="22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="18" t="s">
         <v>9</v>
       </c>
       <c r="I13" s="19" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1202,22 +1202,22 @@
     </row>
     <row r="19" spans="1:9">
       <c r="B19" s="24" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="B20" s="24" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="B21" s="24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="B22" s="24" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="26" spans="1:9" s="2" customFormat="1" ht="14.4">

</xml_diff>